<commit_message>
se ajusta para ver los datos nuevos de analisis
</commit_message>
<xml_diff>
--- a/public/download/RR_Actualización_productos_de_información.xlsx
+++ b/public/download/RR_Actualización_productos_de_información.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iodiaz\OneDrive - Fundacion Accion contra el Hambre\Documentos\MIRESYS\MEAL\respuesta rapida\rr productos de informacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACH\backend\API-REST-LARAVEL\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D6722C-CACA-4A90-BEEB-431CDB8884C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D72F0-AF59-4C91-A8B2-7E6E69237316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{88BF8A4E-949E-40AE-A0AC-7CCFE83A54CB}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="19180" windowHeight="10060" xr2:uid="{88BF8A4E-949E-40AE-A0AC-7CCFE83A54CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos de Información" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,19 +47,7 @@
     <t>Municipio</t>
   </si>
   <si>
-    <t>Fecha de ERN</t>
-  </si>
-  <si>
-    <t>Tipo de Emergencia</t>
-  </si>
-  <si>
     <t>Año</t>
-  </si>
-  <si>
-    <t>Link ERN</t>
-  </si>
-  <si>
-    <t>Link Ficha de Cierre</t>
   </si>
   <si>
     <t>https://reliefweb.int/report/colombia/colombia-evaluacion-rapida-de-necesidades-ern-argelia-cauca-mire-02052024</t>
@@ -69,14 +56,26 @@
     <t>https://reliefweb.int/report/colombia/colombia-ficha-de-cierre-de-emergencias-fce-argelia-cauca-02052024</t>
   </si>
   <si>
-    <t>&lt;respete este formato</t>
+    <t>Tipo de Respuesta</t>
+  </si>
+  <si>
+    <t>Tipo de producto</t>
+  </si>
+  <si>
+    <t>Fecha de Elaboración</t>
+  </si>
+  <si>
+    <t>Enlace</t>
+  </si>
+  <si>
+    <t>por favor respetar este formato</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +112,6 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -148,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -183,7 +175,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -530,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFA0483-B189-465D-81B3-EC694E124512}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,50 +538,50 @@
     <col min="8" max="8" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="H1" t="s">
+        <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="9" t="s">
-        <v>8</v>
+      <c r="H2" s="9" t="s">
+        <v>4</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>9</v>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -598,9 +589,8 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -610,7 +600,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -620,7 +610,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -630,7 +620,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -640,7 +630,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -650,7 +640,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -660,7 +650,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -670,7 +660,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -680,7 +670,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -690,7 +680,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -700,7 +690,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -710,7 +700,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -725,8 +715,8 @@
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{45C8CE25-7E62-4AF1-A7C5-6A6A0B73487C}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{941AB6E3-34B7-4AA0-BEE5-88DF888D58E9}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{45C8CE25-7E62-4AF1-A7C5-6A6A0B73487C}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{941AB6E3-34B7-4AA0-BEE5-88DF888D58E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -784,6 +774,34 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="017991c5-8136-424e-91db-590dc49a3503">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885" xsi:nil="true"/>
+    <_dlc_DocId xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">XU7H42U2DFTR-482029788-401133</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">
+      <Url>https://nohungerforum.sharepoint.com/mi/co/_layouts/15/DocIdRedir.aspx?ID=XU7H42U2DFTR-482029788-401133</Url>
+      <Description>XU7H42U2DFTR-482029788-401133</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F116CB73724D9C41862FD86713FDE4C3" ma:contentTypeVersion="63" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d60833682109817c97cb1e583340a5b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9c62a22c-cb76-48dc-acff-7f03cd5e6885" xmlns:ns3="017991c5-8136-424e-91db-590dc49a3503" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e0157b17ab07458b2a125433d6a1f475" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1091,34 +1109,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="017991c5-8136-424e-91db-590dc49a3503">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885" xsi:nil="true"/>
-    <_dlc_DocId xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">XU7H42U2DFTR-482029788-401133</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">
-      <Url>https://nohungerforum.sharepoint.com/mi/co/_layouts/15/DocIdRedir.aspx?ID=XU7H42U2DFTR-482029788-401133</Url>
-      <Description>XU7H42U2DFTR-482029788-401133</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F028D87A-741E-4A21-9B47-E47A5E09110C}">
   <ds:schemaRefs>
@@ -1128,6 +1118,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0385DDE9-4FF0-41FF-8DD3-5BDE7B2B704E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BFC0B99-E910-47B3-B21A-F7D9BCDA7253}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="017991c5-8136-424e-91db-590dc49a3503"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="9c62a22c-cb76-48dc-acff-7f03cd5e6885"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E39A09B4-8156-44E7-B51D-B38B723153F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1146,25 +1157,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BFC0B99-E910-47B3-B21A-F7D9BCDA7253}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="017991c5-8136-424e-91db-590dc49a3503"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="9c62a22c-cb76-48dc-acff-7f03cd5e6885"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0385DDE9-4FF0-41FF-8DD3-5BDE7B2B704E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
se ajusta para poder exportar excel con productos de infromacion
</commit_message>
<xml_diff>
--- a/public/download/RR_Actualización_productos_de_información.xlsx
+++ b/public/download/RR_Actualización_productos_de_información.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACH\backend\API-REST-LARAVEL\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D72F0-AF59-4C91-A8B2-7E6E69237316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69948739-18F1-42E4-9E8C-21F2E1D65E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="19180" windowHeight="10060" xr2:uid="{88BF8A4E-949E-40AE-A0AC-7CCFE83A54CB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{88BF8A4E-949E-40AE-A0AC-7CCFE83A54CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos de Información" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Código</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Año</t>
   </si>
   <si>
-    <t>https://reliefweb.int/report/colombia/colombia-evaluacion-rapida-de-necesidades-ern-argelia-cauca-mire-02052024</t>
-  </si>
-  <si>
-    <t>https://reliefweb.int/report/colombia/colombia-ficha-de-cierre-de-emergencias-fce-argelia-cauca-02052024</t>
-  </si>
-  <si>
     <t>Tipo de Respuesta</t>
   </si>
   <si>
@@ -65,10 +59,13 @@
     <t>Fecha de Elaboración</t>
   </si>
   <si>
-    <t>Enlace</t>
+    <t>Enlace rr</t>
   </si>
   <si>
-    <t>por favor respetar este formato</t>
+    <t>Enlace rt</t>
+  </si>
+  <si>
+    <t>Tipo de emergencia</t>
   </si>
 </sst>
 </file>
@@ -524,7 +521,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,10 +537,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -555,12 +552,18 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -571,15 +574,8 @@
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="H2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
@@ -714,16 +710,40 @@
   <conditionalFormatting sqref="A2:A15">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{45C8CE25-7E62-4AF1-A7C5-6A6A0B73487C}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{941AB6E3-34B7-4AA0-BEE5-88DF888D58E9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="017991c5-8136-424e-91db-590dc49a3503">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885" xsi:nil="true"/>
+    <_dlc_DocId xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">XU7H42U2DFTR-482029788-401133</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">
+      <Url>https://nohungerforum.sharepoint.com/mi/co/_layouts/15/DocIdRedir.aspx?ID=XU7H42U2DFTR-482029788-401133</Url>
+      <Description>XU7H42U2DFTR-482029788-401133</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -771,34 +791,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="017991c5-8136-424e-91db-590dc49a3503">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885" xsi:nil="true"/>
-    <_dlc_DocId xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">XU7H42U2DFTR-482029788-401133</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="9c62a22c-cb76-48dc-acff-7f03cd5e6885">
-      <Url>https://nohungerforum.sharepoint.com/mi/co/_layouts/15/DocIdRedir.aspx?ID=XU7H42U2DFTR-482029788-401133</Url>
-      <Description>XU7H42U2DFTR-482029788-401133</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1110,22 +1102,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F028D87A-741E-4A21-9B47-E47A5E09110C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0385DDE9-4FF0-41FF-8DD3-5BDE7B2B704E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BFC0B99-E910-47B3-B21A-F7D9BCDA7253}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1134,6 +1110,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
     <ds:schemaRef ds:uri="9c62a22c-cb76-48dc-acff-7f03cd5e6885"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0385DDE9-4FF0-41FF-8DD3-5BDE7B2B704E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F028D87A-741E-4A21-9B47-E47A5E09110C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>